<commit_message>
them api sua pass, profile
</commit_message>
<xml_diff>
--- a/src/main/resources/api.xlsx
+++ b/src/main/resources/api.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
   <si>
     <t>STT</t>
   </si>
@@ -506,6 +506,37 @@
   <si>
     <t>POST 
 http://localhost:8080/api/categories</t>
+  </si>
+  <si>
+    <t>Thay đổi pass</t>
+  </si>
+  <si>
+    <t>Thay đổi password</t>
+  </si>
+  <si>
+    <t>POST http://localhost:8080/api/users/changePass</t>
+  </si>
+  <si>
+    <t>Có token</t>
+  </si>
+  <si>
+    <t>Thông tin user vừa thay đổi pass</t>
+  </si>
+  <si>
+    <t>Thay đổi profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST
+http://localhost:8080/api/users/changeProfile
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file json có dạng
+{"fullname":"tuan", "email":"tuan@gmail.com"
+Ngoài ra có file </t>
+  </si>
+  <si>
+    <t>Thông tin user</t>
   </si>
 </sst>
 </file>
@@ -891,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,24 +1038,50 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2667,7 +2724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>